<commit_message>
Data Provider for parameterized test
</commit_message>
<xml_diff>
--- a/BestCruiseFramework/src/test/resources/excel/testdata.xlsx
+++ b/BestCruiseFramework/src/test/resources/excel/testdata.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\eclipse-workspace\BestCruiseFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\git\BestCruiseFramework\BestCruiseFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="2700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="2700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="singleCruiseTest" sheetId="1" r:id="rId1"/>
+    <sheet name="parameterizedSearchTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>Y</t>
   </si>
@@ -81,6 +82,51 @@
   </si>
   <si>
     <t>cruiseLisbon2504Kiel0205</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>initialPort</t>
+  </si>
+  <si>
+    <t>minCruiseLength</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>BritishIslands</t>
+  </si>
+  <si>
+    <t>GreatBritain</t>
+  </si>
+  <si>
+    <t>Genoa</t>
+  </si>
+  <si>
+    <t>NearEast</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Marseille</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>AnyCountry</t>
+  </si>
+  <si>
+    <t>Rome</t>
+  </si>
+  <si>
+    <t>20 июнь</t>
   </si>
 </sst>
 </file>
@@ -403,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -538,4 +584,107 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.46484375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.46484375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ref for parallel execution
</commit_message>
<xml_diff>
--- a/BestCruiseFramework/src/test/resources/excel/testdata.xlsx
+++ b/BestCruiseFramework/src/test/resources/excel/testdata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Y</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>20 июнь</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Savona</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -561,7 +567,7 @@
         <v>40000</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
@@ -588,10 +594,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -604,7 +610,7 @@
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -623,8 +629,11 @@
       <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>24</v>
       </c>
@@ -643,8 +652,11 @@
       <c r="F2" s="1">
         <v>60000</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -663,8 +675,11 @@
       <c r="F3" s="1">
         <v>60000</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -681,7 +696,33 @@
         <v>33</v>
       </c>
       <c r="F4" s="1">
-        <v>100000</v>
+        <v>60000</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1">
+        <v>60000</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>